<commit_message>
Clean across survey analysis
</commit_message>
<xml_diff>
--- a/Across surveys/TM - Ind wise employment share 27Dec24.xlsx
+++ b/Across surveys/TM - Ind wise employment share 27Dec24.xlsx
@@ -279,16 +279,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,34 +576,34 @@
       <selection activeCell="K12" sqref="K3:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="23.36328125" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -630,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
@@ -653,12 +653,12 @@
       <c r="I4" s="1">
         <v>72133</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="22">
         <v>46.073544923974737</v>
       </c>
-      <c r="K4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="7" t="s">
         <v>16</v>
@@ -681,12 +681,12 @@
       <c r="I5" s="1">
         <v>30139</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="22">
         <v>13.224767358795809</v>
       </c>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="7" t="s">
         <v>6</v>
@@ -709,12 +709,12 @@
       <c r="I6" s="1">
         <v>20917</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="22">
         <v>11.976432368646032</v>
       </c>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
@@ -737,12 +737,12 @@
       <c r="I7" s="1">
         <v>21854</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="22">
         <v>11.441682959445762</v>
       </c>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K7" s="21"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -765,12 +765,12 @@
       <c r="I8" s="1">
         <v>22631</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="22">
         <v>10.232307537018528</v>
       </c>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" s="21"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
@@ -793,12 +793,12 @@
       <c r="I9" s="1">
         <v>9067</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="22">
         <v>4.2769634701307</v>
       </c>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="7" t="s">
         <v>10</v>
@@ -821,12 +821,12 @@
       <c r="I10" s="1">
         <v>4440</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="22">
         <v>1.9975747540236157</v>
       </c>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
         <v>11</v>
@@ -849,12 +849,12 @@
       <c r="I11" s="1">
         <v>1322</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="22">
         <v>0.54405713238657238</v>
       </c>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -877,37 +877,37 @@
       <c r="I12" s="1">
         <v>567</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="22">
         <v>0.23266949557825234</v>
       </c>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K24" s="22"/>
-    </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K25" s="22"/>
+      <c r="K12" s="21"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -923,51 +923,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.08984375" customWidth="1"/>
-    <col min="14" max="14" width="5.1796875" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="18" width="8.7265625" style="10"/>
+    <col min="17" max="17" width="12" style="10" customWidth="1"/>
+    <col min="18" max="18" width="14" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
       <c r="Q2"/>
       <c r="R2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1030,7 +1031,7 @@
       <c r="J4" s="1">
         <v>70591</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="23">
         <f>I4/SUM($I$4:$I$89)</f>
         <v>0.45242197758435582</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>0.4607354492397473</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>2.3266949557825237E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>0.11441682959445762</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>2.7288111164227489E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>2.7117602074429757E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>0.1197643236864603</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>0.10232307537018526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>4.9555343010168913E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1374,7 +1375,7 @@
         <v>1.9975747540236153E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>1.3513300881551393E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1456,7 +1457,7 @@
         <v>1.0521308557088918E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>2.1574905981164259E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>6.7496493927049163E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>9.1860046116270713E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>1.4176102902481044E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>3.0434562090938304E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>1.3482190818173574E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>2.2352819230669796E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>1.6687090320886333E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>1.3104691491323111E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>7.3436809990343821E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>3.6064698060326063E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1956,7 +1957,7 @@
         <v>6.1172803438427912E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1986,7 +1987,7 @@
         <v>1.1951954947196284E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2016,7 +2017,7 @@
         <v>2.395016512098354E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>2.3595871387045763E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>2.5902679638501176E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>1.0825073401024953E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>5.3933099700187205E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>6.1116144589737735E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>3.1115293717997603E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>2.7288111164227489E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>9.413338019058793E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>1.7839454084404122E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2316,7 +2317,7 @@
         <v>1.5718408496646918E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2346,7 +2347,7 @@
         <v>2.0191015028363059E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>9.6481955085790785E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>9.5473089033450455E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -2436,7 +2437,7 @@
         <v>1.3735059697324475E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>8.8720187320125866E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>1.5412987061330917E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>47</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>7.8038069576841756E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>49</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>3.7814100400290103E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>50</v>
       </c>
@@ -2586,7 +2587,7 @@
         <v>2.9100851972774287E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>51</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>1.4987111842690098E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>52</v>
       </c>
@@ -2646,7 +2647,7 @@
         <v>3.2524936963892626E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>53</v>
       </c>
@@ -2676,7 +2677,7 @@
         <v>1.262160966472985E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>55</v>
       </c>
@@ -2706,7 +2707,7 @@
         <v>1.5521234181651591E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>56</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>1.8423624122070995E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>58</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>4.167972500339644E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>59</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>5.5519395308161574E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>60</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>1.1627141312442718E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>61</v>
       </c>
@@ -2856,7 +2857,7 @@
         <v>9.9272236963867332E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>62</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>9.8921956327302375E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>63</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>1.5401202629424762E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>64</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>8.4323373172441405E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>65</v>
       </c>
@@ -2976,7 +2977,7 @@
         <v>9.6271923643667374E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>66</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>1.1262520034081049E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>68</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>2.1574905981164259E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>69</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>3.0239373403268674E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>70</v>
       </c>
@@ -3096,7 +3097,7 @@
         <v>2.3930232770051244E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>71</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>6.1730757109181554E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>72</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>1.1827415792707096E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>73</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>2.8453811344227839E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>74</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>2.0183882746302364E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>75</v>
       </c>
@@ -3246,7 +3247,7 @@
         <v>4.479016075861356E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>77</v>
       </c>
@@ -3276,7 +3277,7 @@
         <v>1.945793054903636E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>78</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>9.8551020601889638E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>79</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>5.7435411560947263E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>80</v>
       </c>
@@ -3366,7 +3367,7 @@
         <v>1.9055346510692952E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>81</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>9.7052670786578366E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>82</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>2.804285876159988E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>84</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>1.4176102902481044E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>85</v>
       </c>
@@ -3486,7 +3487,7 @@
         <v>3.0434562090938304E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>86</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>1.1572346366797735E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>87</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>3.0210254673042201E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>88</v>
       </c>
@@ -3576,7 +3577,7 @@
         <v>1.6077419046454172E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>90</v>
       </c>
@@ -3606,7 +3607,7 @@
         <v>1.5214241742340354E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>91</v>
       </c>
@@ -3636,7 +3637,7 @@
         <v>1.0473042977927769E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>92</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>2.3278247092609378E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>93</v>
       </c>
@@ -3696,7 +3697,7 @@
         <v>3.7634484812757276E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>94</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>2.9612284145073349E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>95</v>
       </c>
@@ -3756,7 +3757,7 @@
         <v>4.686550268292582E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>96</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>9.0393116380864166E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>97</v>
       </c>
@@ -3816,7 +3817,7 @@
         <v>1.3104691491323111E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>99</v>
       </c>
@@ -3835,7 +3836,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>